<commit_message>
Not needed additional wires for CLC.
</commit_message>
<xml_diff>
--- a/zDocuments/CS-1325_R00_Communication.xlsx
+++ b/zDocuments/CS-1325_R00_Communication.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3071EE3D-E514-472D-B71D-E27AB4B600AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F500F809-13FE-4829-BAFC-86F099C787A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="884">
   <si>
     <t>RA0</t>
   </si>
@@ -2737,6 +2737,12 @@
   </si>
   <si>
     <t># iTempTRIP</t>
+  </si>
+  <si>
+    <t>Not needed WIRE between RC1 (TP2) and RD3 (#FltOut)</t>
+  </si>
+  <si>
+    <t>Not needed WIRE between RD5 (TP6) and RD4 (TP5)</t>
   </si>
 </sst>
 </file>
@@ -3403,11 +3409,26 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3415,13 +3436,7 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3439,22 +3454,13 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -14242,11 +14248,11 @@
       <c r="A1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="142" t="s">
+      <c r="E1" s="157" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
       <c r="M1" s="14" t="s">
         <v>49</v>
       </c>
@@ -14302,18 +14308,18 @@
       <c r="E3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="143" t="s">
+      <c r="F3" s="158" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143" t="s">
+      <c r="G3" s="158"/>
+      <c r="H3" s="158" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="143"/>
-      <c r="J3" s="144" t="s">
+      <c r="I3" s="158"/>
+      <c r="J3" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="145"/>
+      <c r="K3" s="150"/>
       <c r="M3" s="15" t="s">
         <v>285</v>
       </c>
@@ -14333,16 +14339,16 @@
       <c r="E4" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="146" t="s">
+      <c r="F4" s="159" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="146"/>
-      <c r="H4" s="147" t="s">
+      <c r="G4" s="159"/>
+      <c r="H4" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="I4" s="148"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="148"/>
+      <c r="I4" s="144"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="144"/>
       <c r="M4" s="15" t="s">
         <v>286</v>
       </c>
@@ -14460,14 +14466,14 @@
       <c r="F8" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="151" t="s">
+      <c r="G8" s="154" t="s">
         <v>84</v>
       </c>
-      <c r="H8" s="152"/>
-      <c r="I8" s="144" t="s">
+      <c r="H8" s="155"/>
+      <c r="I8" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="145"/>
+      <c r="J8" s="150"/>
       <c r="L8" s="28"/>
       <c r="M8" s="15" t="s">
         <v>290</v>
@@ -14491,10 +14497,10 @@
       <c r="F9" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="147"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="147"/>
-      <c r="J9" s="148"/>
+      <c r="G9" s="143"/>
+      <c r="H9" s="144"/>
+      <c r="I9" s="143"/>
+      <c r="J9" s="144"/>
       <c r="L9" s="28"/>
       <c r="M9" s="15" t="s">
         <v>291</v>
@@ -14580,10 +14586,10 @@
       <c r="F12" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="144" t="s">
+      <c r="G12" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="145"/>
+      <c r="H12" s="150"/>
       <c r="I12" s="28" t="s">
         <v>92</v>
       </c>
@@ -14612,8 +14618,8 @@
       <c r="F13" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="G13" s="147"/>
-      <c r="H13" s="148"/>
+      <c r="G13" s="143"/>
+      <c r="H13" s="144"/>
       <c r="L13" s="13"/>
       <c r="M13" s="15" t="s">
         <v>295</v>
@@ -14645,11 +14651,11 @@
       <c r="D15" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="153" t="s">
+      <c r="E15" s="156" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
+      <c r="F15" s="156"/>
+      <c r="G15" s="156"/>
       <c r="L15" s="13"/>
       <c r="M15" s="15" t="s">
         <v>297</v>
@@ -14712,18 +14718,18 @@
       <c r="E17" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="149" t="s">
+      <c r="F17" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="150"/>
-      <c r="H17" s="149" t="s">
+      <c r="G17" s="153"/>
+      <c r="H17" s="152" t="s">
         <v>98</v>
       </c>
-      <c r="I17" s="150"/>
-      <c r="J17" s="144" t="s">
+      <c r="I17" s="153"/>
+      <c r="J17" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="K17" s="145"/>
+      <c r="K17" s="150"/>
       <c r="L17" s="13"/>
       <c r="M17" s="15" t="s">
         <v>299</v>
@@ -14744,16 +14750,16 @@
       <c r="E18" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="147" t="s">
+      <c r="F18" s="143" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="148"/>
-      <c r="H18" s="147" t="s">
+      <c r="G18" s="144"/>
+      <c r="H18" s="143" t="s">
         <v>280</v>
       </c>
-      <c r="I18" s="148"/>
-      <c r="J18" s="147"/>
-      <c r="K18" s="148"/>
+      <c r="I18" s="144"/>
+      <c r="J18" s="143"/>
+      <c r="K18" s="144"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.5">
@@ -14860,14 +14866,14 @@
       <c r="F22" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="149" t="s">
+      <c r="G22" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="H22" s="150"/>
-      <c r="I22" s="144" t="s">
+      <c r="H22" s="153"/>
+      <c r="I22" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="J22" s="145"/>
+      <c r="J22" s="150"/>
       <c r="L22" s="13"/>
       <c r="M22" s="56" t="s">
         <v>313</v>
@@ -14891,10 +14897,10 @@
       <c r="F23" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="G23" s="147"/>
-      <c r="H23" s="148"/>
-      <c r="I23" s="147"/>
-      <c r="J23" s="148"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="144"/>
+      <c r="I23" s="143"/>
+      <c r="J23" s="144"/>
       <c r="L23" s="13"/>
       <c r="M23" s="56" t="s">
         <v>314</v>
@@ -14988,10 +14994,10 @@
       <c r="F26" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="G26" s="144" t="s">
+      <c r="G26" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="145"/>
+      <c r="H26" s="150"/>
       <c r="I26" s="28" t="s">
         <v>92</v>
       </c>
@@ -15023,8 +15029,8 @@
       <c r="F27" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="147"/>
-      <c r="H27" s="148"/>
+      <c r="G27" s="143"/>
+      <c r="H27" s="144"/>
       <c r="L27" s="13"/>
       <c r="M27" s="56" t="s">
         <v>318</v>
@@ -15057,11 +15063,11 @@
       <c r="B29" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E29" s="156" t="s">
+      <c r="E29" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="F29" s="156"/>
-      <c r="G29" s="156"/>
+      <c r="F29" s="151"/>
+      <c r="G29" s="151"/>
       <c r="L29" s="13"/>
       <c r="M29" s="56" t="s">
         <v>320</v>
@@ -15124,18 +15130,18 @@
       <c r="E31" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="154" t="s">
+      <c r="F31" s="147" t="s">
         <v>110</v>
       </c>
-      <c r="G31" s="155"/>
-      <c r="H31" s="154" t="s">
+      <c r="G31" s="148"/>
+      <c r="H31" s="147" t="s">
         <v>84</v>
       </c>
-      <c r="I31" s="155"/>
-      <c r="J31" s="144" t="s">
+      <c r="I31" s="148"/>
+      <c r="J31" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="K31" s="145"/>
+      <c r="K31" s="150"/>
       <c r="L31" s="13"/>
       <c r="M31" s="56" t="s">
         <v>322</v>
@@ -15150,16 +15156,16 @@
       <c r="E32" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="147" t="s">
+      <c r="F32" s="143" t="s">
         <v>73</v>
       </c>
-      <c r="G32" s="148"/>
-      <c r="H32" s="147" t="s">
+      <c r="G32" s="144"/>
+      <c r="H32" s="143" t="s">
         <v>73</v>
       </c>
-      <c r="I32" s="148"/>
-      <c r="J32" s="147"/>
-      <c r="K32" s="148"/>
+      <c r="I32" s="144"/>
+      <c r="J32" s="143"/>
+      <c r="K32" s="144"/>
       <c r="M32" s="56" t="s">
         <v>323</v>
       </c>
@@ -15268,18 +15274,18 @@
       <c r="E36" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="F36" s="154" t="s">
+      <c r="F36" s="147" t="s">
         <v>110</v>
       </c>
-      <c r="G36" s="155"/>
-      <c r="H36" s="157" t="s">
+      <c r="G36" s="148"/>
+      <c r="H36" s="145" t="s">
         <v>84</v>
       </c>
-      <c r="I36" s="158"/>
-      <c r="J36" s="144" t="s">
+      <c r="I36" s="146"/>
+      <c r="J36" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="K36" s="145"/>
+      <c r="K36" s="150"/>
       <c r="L36" s="13"/>
       <c r="M36" s="56" t="s">
         <v>326</v>
@@ -15297,14 +15303,14 @@
       <c r="E37" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="F37" s="147" t="s">
+      <c r="F37" s="143" t="s">
         <v>73</v>
       </c>
-      <c r="G37" s="148"/>
-      <c r="H37" s="147"/>
-      <c r="I37" s="148"/>
-      <c r="J37" s="147"/>
-      <c r="K37" s="148"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="143"/>
+      <c r="I37" s="144"/>
+      <c r="J37" s="143"/>
+      <c r="K37" s="144"/>
       <c r="L37" s="13"/>
       <c r="M37" s="56" t="s">
         <v>327</v>
@@ -15385,10 +15391,10 @@
       <c r="F40" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="144" t="s">
+      <c r="G40" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="H40" s="145"/>
+      <c r="H40" s="150"/>
       <c r="I40" s="28" t="s">
         <v>92</v>
       </c>
@@ -15407,8 +15413,8 @@
       <c r="F41" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="G41" s="147"/>
-      <c r="H41" s="148"/>
+      <c r="G41" s="143"/>
+      <c r="H41" s="144"/>
       <c r="L41" s="13"/>
       <c r="M41" s="14" t="s">
         <v>49</v>
@@ -15572,11 +15578,28 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="J37:K37"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="J36:K36"/>
@@ -15591,28 +15614,11 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="G26:H26"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="G40:H40"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -15624,8 +15630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7649C711-B6D3-4AA5-828E-893E07D95988}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
@@ -15977,17 +15983,8 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="C18" s="13" t="s">
-        <v>871</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>872</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>873</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>874</v>
+      <c r="C18" s="19" t="s">
+        <v>882</v>
       </c>
       <c r="J18" s="13" t="s">
         <v>837</v>
@@ -16007,8 +16004,9 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A19" s="46"/>
-      <c r="B19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="C19" s="19" t="s">
+        <v>883</v>
+      </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13" t="s">
@@ -16018,19 +16016,6 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A20" s="46"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="159" t="s">
-        <v>880</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>879</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>844</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>875</v>
-      </c>
       <c r="I20" s="140" t="s">
         <v>857</v>
       </c>
@@ -16057,21 +16042,6 @@
       <c r="A21" s="53" t="s">
         <v>254</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>878</v>
-      </c>
-      <c r="C21" s="159">
-        <v>0</v>
-      </c>
-      <c r="D21" s="17">
-        <v>1</v>
-      </c>
-      <c r="E21" s="17">
-        <v>0</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>876</v>
-      </c>
       <c r="J21" s="13">
         <v>0</v>
       </c>
@@ -16090,19 +16060,6 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A22" s="55"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="159">
-        <v>1</v>
-      </c>
-      <c r="D22" s="17">
-        <v>0</v>
-      </c>
-      <c r="E22" s="17">
-        <v>1</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>334</v>
-      </c>
       <c r="J22" s="141">
         <v>0</v>
       </c>
@@ -16123,8 +16080,6 @@
       <c r="A23" s="50" t="s">
         <v>264</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="F23" s="13"/>
       <c r="J23" s="13">
         <v>1</v>
       </c>
@@ -16145,18 +16100,17 @@
       <c r="A24" s="50" t="s">
         <v>264</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="159" t="s">
-        <v>877</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>879</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>844</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>875</v>
+      <c r="C24" s="13" t="s">
+        <v>871</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>872</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>873</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>874</v>
       </c>
       <c r="J24" s="13">
         <v>1</v>
@@ -16178,18 +16132,8 @@
       <c r="A25" s="50" t="s">
         <v>264</v>
       </c>
-      <c r="C25" s="159">
-        <v>0</v>
-      </c>
-      <c r="D25" s="17">
-        <v>0</v>
-      </c>
-      <c r="E25" s="17">
-        <v>1</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>334</v>
-      </c>
+      <c r="B25" s="13"/>
+      <c r="F25" s="13"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13" t="s">
         <v>848</v>
@@ -16204,38 +16148,52 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A26" s="55"/>
-      <c r="B26" s="28" t="s">
-        <v>878</v>
-      </c>
-      <c r="C26" s="159">
-        <v>1</v>
-      </c>
-      <c r="D26" s="17">
-        <v>1</v>
-      </c>
-      <c r="E26" s="17">
-        <v>0</v>
+      <c r="B26" s="13"/>
+      <c r="C26" s="142" t="s">
+        <v>880</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>879</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>844</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A27" s="55"/>
+      <c r="B27" s="28" t="s">
+        <v>878</v>
+      </c>
+      <c r="C27" s="142">
+        <v>0</v>
+      </c>
+      <c r="D27" s="17">
+        <v>1</v>
+      </c>
+      <c r="E27" s="17">
+        <v>0</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A28" s="55"/>
-      <c r="C28" s="159" t="s">
-        <v>881</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>879</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>844</v>
+      <c r="B28" s="28"/>
+      <c r="C28" s="142">
+        <v>1</v>
+      </c>
+      <c r="D28" s="17">
+        <v>0</v>
+      </c>
+      <c r="E28" s="17">
+        <v>1</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>875</v>
+        <v>334</v>
       </c>
       <c r="I28" s="140" t="s">
         <v>859</v>
@@ -16254,21 +16212,8 @@
       <c r="A29" s="50" t="s">
         <v>259</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>878</v>
-      </c>
-      <c r="C29" s="159">
-        <v>0</v>
-      </c>
-      <c r="D29" s="17">
-        <v>1</v>
-      </c>
-      <c r="E29" s="17">
-        <v>0</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>876</v>
-      </c>
+      <c r="B29" s="13"/>
+      <c r="F29" s="13"/>
       <c r="J29" s="17">
         <v>0</v>
       </c>
@@ -16278,17 +16223,18 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A30" s="55"/>
-      <c r="C30" s="159">
-        <v>1</v>
-      </c>
-      <c r="D30" s="17">
-        <v>0</v>
-      </c>
-      <c r="E30" s="17">
-        <v>1</v>
+      <c r="B30" s="13"/>
+      <c r="C30" s="142" t="s">
+        <v>877</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>879</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>844</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>334</v>
+        <v>875</v>
       </c>
       <c r="J30" s="17">
         <v>1</v>
@@ -16301,25 +16247,60 @@
       <c r="A31" s="41" t="s">
         <v>309</v>
       </c>
-      <c r="F31" s="13"/>
+      <c r="C31" s="142">
+        <v>0</v>
+      </c>
+      <c r="D31" s="17">
+        <v>0</v>
+      </c>
+      <c r="E31" s="17">
+        <v>1</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>334</v>
+      </c>
       <c r="K31" s="14" t="s">
         <v>848</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A32" s="46"/>
-      <c r="F32" s="13"/>
+      <c r="B32" s="28" t="s">
+        <v>878</v>
+      </c>
+      <c r="C32" s="142">
+        <v>1</v>
+      </c>
+      <c r="D32" s="17">
+        <v>1</v>
+      </c>
+      <c r="E32" s="17">
+        <v>0</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A33" s="41"/>
-      <c r="F33" s="13"/>
       <c r="K33" s="13" t="s">
         <v>844</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A34" s="41"/>
-      <c r="F34" s="13"/>
+      <c r="C34" s="142" t="s">
+        <v>881</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>879</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>875</v>
+      </c>
       <c r="J34" s="13"/>
       <c r="K34" s="13" t="s">
         <v>16</v>
@@ -16327,7 +16308,21 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A35" s="41"/>
-      <c r="F35" s="13"/>
+      <c r="B35" s="28" t="s">
+        <v>878</v>
+      </c>
+      <c r="C35" s="142">
+        <v>0</v>
+      </c>
+      <c r="D35" s="17">
+        <v>1</v>
+      </c>
+      <c r="E35" s="17">
+        <v>0</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>876</v>
+      </c>
       <c r="I35" s="140" t="s">
         <v>858</v>
       </c>
@@ -16343,6 +16338,18 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A36" s="41"/>
+      <c r="C36" s="142">
+        <v>1</v>
+      </c>
+      <c r="D36" s="17">
+        <v>0</v>
+      </c>
+      <c r="E36" s="17">
+        <v>1</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>334</v>
+      </c>
       <c r="J36" s="16">
         <v>0</v>
       </c>

</xml_diff>